<commit_message>
[0020] Listado jornales, buscador por obra y fechas
</commit_message>
<xml_diff>
--- a/estructuraTablas.xlsx
+++ b/estructuraTablas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\proyectofinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D892F6-7FFB-44BD-B04C-B09AC9C9AEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62877382-63E2-4E66-9448-80BDCE9397CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{4C979411-F035-452A-A459-0C87E3674971}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4C979411-F035-452A-A459-0C87E3674971}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
   <si>
     <t>PERSONA</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>motivo</t>
+  </si>
+  <si>
+    <t>confirmado</t>
   </si>
 </sst>
 </file>
@@ -289,7 +295,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,28 +633,28 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.41796875" customWidth="1"/>
-    <col min="2" max="2" width="12.9453125" customWidth="1"/>
-    <col min="3" max="3" width="14.1015625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="20.20703125" customWidth="1"/>
-    <col min="6" max="6" width="13.20703125" customWidth="1"/>
-    <col min="7" max="7" width="19.5234375" customWidth="1"/>
-    <col min="8" max="8" width="15.578125" customWidth="1"/>
-    <col min="9" max="9" width="12.68359375" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -677,12 +683,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -704,12 +710,12 @@
       <c r="G5" s="3"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -731,12 +737,12 @@
       <c r="G9" s="3"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -761,13 +767,16 @@
       <c r="H12" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I12" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -781,12 +790,12 @@
       <c r="G17" s="3"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
@@ -809,15 +818,15 @@
         <v>22</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
@@ -835,12 +844,12 @@
       <c r="G27" s="3"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
@@ -854,12 +863,12 @@
       <c r="G31" s="3"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
@@ -881,12 +890,12 @@
       <c r="G35" s="3"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
@@ -913,19 +922,19 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.3125" customWidth="1"/>
-    <col min="2" max="2" width="14.1015625" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -951,7 +960,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -977,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1003,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1029,12 +1038,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -1042,7 +1051,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1050,7 +1059,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1058,7 +1067,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1066,12 +1075,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
@@ -1097,7 +1106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>

</xml_diff>